<commit_message>
Adding values from excel to ShareSkill
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MVPProject\Competitiontask1\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7D007D-068B-4289-BD0B-2631490D771A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0926889-26DF-434E-83DA-9192FEF57055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
-    <sheet name="SignIn" sheetId="1" r:id="rId2"/>
-    <sheet name="Profile" sheetId="2" r:id="rId3"/>
+    <sheet name="&quot;ManageListings" sheetId="5" r:id="rId2"/>
+    <sheet name="SignIn" sheetId="1" r:id="rId3"/>
+    <sheet name="ShareSkill" sheetId="4" r:id="rId4"/>
+    <sheet name="Profile" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Url</t>
   </si>
@@ -124,6 +126,87 @@
   </si>
   <si>
     <t>Amma260872</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>SubCategory</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>LocationType</t>
+  </si>
+  <si>
+    <t>Startdate</t>
+  </si>
+  <si>
+    <t>Enddate</t>
+  </si>
+  <si>
+    <t>Selectday</t>
+  </si>
+  <si>
+    <t>Starttime</t>
+  </si>
+  <si>
+    <t>Endtime</t>
+  </si>
+  <si>
+    <t>SkillTrade</t>
+  </si>
+  <si>
+    <t>Skill-Exchange</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>Would like to provide selenium training for beginners</t>
+  </si>
+  <si>
+    <t>Programming &amp; Tech</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>One-off service</t>
+  </si>
+  <si>
+    <t>On-site</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Performance Testing</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Deleteaction</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -176,10 +259,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -577,11 +662,46 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C435061D-5197-4A8C-9AE0-B97AB37D0BF9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -624,7 +744,127 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AED40C2-E387-420A-8307-8C19194F1444}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="39.26953125" customWidth="1"/>
+    <col min="8" max="8" width="16.08984375" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="3">
+        <v>44663</v>
+      </c>
+      <c r="I2" s="3">
+        <v>44724</v>
+      </c>
+      <c r="J2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>

</xml_diff>